<commit_message>
1st round of Settings Scr dev and Main Scr modif
Settings Screen: created first general layout

- TODO: update total_timing and slots values only when the save button
  is pressed

Main Screen: modified general layout:
- Suppressed the 4 slots container to be able to have more than 4 slots
  and save space
- Added big text frame at the top with the current slot's name
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2903" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5508" uniqueCount="148">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -426,6 +426,39 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KEYZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NUM OF SLOTS:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IP DEV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01</t>
   </si>
 </sst>
 </file>
@@ -1928,7 +1961,7 @@
       <c r="G11"/>
       <c r="H11"/>
       <c r="I11" t="s">
-        <v>44</v>
+        <v>106</v>
       </c>
       <c r="J11"/>
       <c r="L11" s="15"/>
@@ -1941,7 +1974,7 @@
         <v>62</v>
       </c>
       <c r="D12">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="E12">
         <v>4</v>
@@ -2321,7 +2354,7 @@
         <v>48</v>
       </c>
       <c r="F21" t="s">
-        <v>118</v>
+        <v>95</v>
       </c>
     </row>
     <row r="22">
@@ -2338,7 +2371,7 @@
         <v>48</v>
       </c>
       <c r="F22" t="s">
-        <v>99</v>
+        <v>147</v>
       </c>
     </row>
     <row r="23">
@@ -2406,7 +2439,7 @@
         <v>48</v>
       </c>
       <c r="F26" t="s">
-        <v>52</v>
+        <v>135</v>
       </c>
     </row>
     <row r="27">
@@ -2440,7 +2473,7 @@
         <v>48</v>
       </c>
       <c r="F28" t="s">
-        <v>52</v>
+        <v>135</v>
       </c>
     </row>
     <row r="29">
@@ -2457,7 +2490,7 @@
         <v>48</v>
       </c>
       <c r="F29" t="s">
-        <v>60</v>
+        <v>144</v>
       </c>
     </row>
     <row r="30">
@@ -2509,6 +2542,91 @@
       </c>
       <c r="F32" t="s">
         <v>135</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="B33" t="s">
+        <v>137</v>
+      </c>
+      <c r="C33" t="s">
+        <v>67</v>
+      </c>
+      <c r="D33" t="s">
+        <v>47</v>
+      </c>
+      <c r="E33" t="s">
+        <v>48</v>
+      </c>
+      <c r="F33" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="B34" t="s">
+        <v>139</v>
+      </c>
+      <c r="C34" t="s">
+        <v>67</v>
+      </c>
+      <c r="D34" t="s">
+        <v>47</v>
+      </c>
+      <c r="E34" t="s">
+        <v>48</v>
+      </c>
+      <c r="F34" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="B35" t="s">
+        <v>141</v>
+      </c>
+      <c r="C35" t="s">
+        <v>120</v>
+      </c>
+      <c r="D35" t="s">
+        <v>47</v>
+      </c>
+      <c r="E35" t="s">
+        <v>48</v>
+      </c>
+      <c r="F35" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="B36" t="s">
+        <v>142</v>
+      </c>
+      <c r="C36" t="s">
+        <v>120</v>
+      </c>
+      <c r="D36" t="s">
+        <v>47</v>
+      </c>
+      <c r="E36" t="s">
+        <v>48</v>
+      </c>
+      <c r="F36" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="B37" t="s">
+        <v>145</v>
+      </c>
+      <c r="C37" t="s">
+        <v>120</v>
+      </c>
+      <c r="D37" t="s">
+        <v>47</v>
+      </c>
+      <c r="E37" t="s">
+        <v>48</v>
+      </c>
+      <c r="F37" t="s">
+        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>